<commit_message>
feat: add fuxtion upto `XLOOKUP` in the excel formulas and function learning tutorial
</commit_message>
<xml_diff>
--- a/sample-data-fx.xlsx
+++ b/sample-data-fx.xlsx
@@ -5,18 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Excel\Excel-function-and-formulas-tutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AEF3BA4-F850-46FA-8E39-FE8C9ACCB126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B75531-E3BE-4F31-936B-CDBBBB1C5C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{26D4546B-D2A1-4444-8EAF-A6228F96F0C1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{26D4546B-D2A1-4444-8EAF-A6228F96F0C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Concepts" sheetId="2" r:id="rId1"/>
     <sheet name="Data" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet1!$A$17:$M$17</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,8 +40,9 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
+  <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -49,16 +53,30 @@
       </extLst>
     </bk>
   </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2403" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2443" uniqueCount="794">
   <si>
     <t>Emp ID</t>
   </si>
@@ -2377,6 +2395,189 @@
   </si>
   <si>
     <t>Fixed Term head count</t>
+  </si>
+  <si>
+    <r>
+      <t>DIPARTMENT BASED CALCULATIONS: [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="22"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>COUNTIFS, SUMIFS,AVERAGEIFS</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="22"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALL EMPLOYEES WITH SALARY GREATER THAN 100 K :(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="22"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FILTER, =STAFF[HEADERS]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="22"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>COLUMNS 1,2,3,5,6: NAMES, DIPARTMENT, SLARAY</t>
+  </si>
+  <si>
+    <r>
+      <t>ALL EMPLOYEES WITH SALARY GREATER THAN 100 K COLUMN :(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FILTER</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, =STAFF[HEADERS],CHOOSECOLS)</t>
+    </r>
+  </si>
+  <si>
+    <t>NOT WORKING IN THIS EXCEL THE FORMULA IS =CHOOSECOLS(FILTER(staff,staff[Salary]&gt;=F67),1,2,3,5,6)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ALL </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FEMALE</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> EMPLOYEES WITH SALARY GREATER THAN 100 K  :(FILTER [MULTIPLE CONDITION], =STAFF[HEADERS],CHOOSECOLS)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ALL </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FEMALE</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> EMPLOYEES WITH SALARY GREATER THAN 100 K AND JOINED AFTER 2019  :(FILTER [MULTIPLE CONDITION], =STAFF[HEADERS],CHOOSECOLS)</t>
+    </r>
+  </si>
+  <si>
+    <t>ALL EMP</t>
+  </si>
+  <si>
+    <t>LOWEST SALARY</t>
+  </si>
+  <si>
+    <t>HIGHEST SALARY</t>
+  </si>
+  <si>
+    <t>TOP 5 SALARY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lowest, highest and top 5 salary values: (MIN, MAX, LARGE, MINIFS) </t>
+  </si>
+  <si>
+    <t>TAKE DOESN’T WORK IN THIS EXCEL SO EQ IS =TAKE(SORT(staff[Salary],,-1),5)</t>
+  </si>
+  <si>
+    <t>count :</t>
+  </si>
+  <si>
+    <t>Employee details lookup: (VLOOKUP, INDEX + MATCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emp ID </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOP 5 SALARY (diff func) </t>
+  </si>
+  <si>
+    <t>Employee details lookup: (XLOOKUP, IFERROR)</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>With xlookup</t>
+  </si>
+  <si>
+    <t>No employes so blank</t>
   </si>
 </sst>
 </file>
@@ -2388,7 +2589,7 @@
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2438,8 +2639,86 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2476,8 +2755,20 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -2534,12 +2825,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2610,6 +2925,48 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -2749,6 +3106,64 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>13</v>
+    <v>3</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3075,7 +3490,7 @@
   <dimension ref="A1:N265"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4547,8 +4962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE182796-6443-4558-9B87-909B73329DFC}">
   <dimension ref="A1:O267"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -15287,360 +15702,4161 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D145AB91-9B7A-4E90-B667-24217E8EC446}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:S278"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="B158" sqref="B158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:17" ht="28.8">
+      <c r="A1" s="34" t="s">
+        <v>773</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B2" s="26" t="s">
         <v>768</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D2" s="26" t="s">
         <v>769</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E2" s="26" t="s">
         <v>770</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F2" s="26" t="s">
         <v>771</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G2" s="26" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+    <row r="3" spans="1:17">
+      <c r="A3" t="s">
         <v>36</v>
-      </c>
-      <c r="B2">
-        <f>COUNTIF(staff[Department],A2)</f>
-        <v>24</v>
-      </c>
-      <c r="C2" s="27" cm="1">
-        <f t="array" ref="C2:C13">SUMIFS(staff[Salary],staff[Department],A2:A13)</f>
-        <v>2013215.1600000001</v>
-      </c>
-      <c r="D2" s="27">
-        <f>AVERAGEIFS(staff[Salary],staff[Department],A2)</f>
-        <v>83883.965000000011</v>
-      </c>
-      <c r="E2">
-        <f>COUNTIFS(staff[Employee type],"Permanent",staff[Department],A2)</f>
-        <v>11</v>
-      </c>
-      <c r="F2" cm="1">
-        <f t="array" ref="F2:F13">COUNTIFS(staff[Employee type],"Temporary",staff[Department],A2:A13)</f>
-        <v>7</v>
-      </c>
-      <c r="G2" cm="1">
-        <f t="array" ref="G2:G13">COUNTIFS(staff[Employee type],"Fixed Term",staff[Department],A2:A13)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>25</v>
       </c>
       <c r="B3">
         <f>COUNTIF(staff[Department],A3)</f>
-        <v>26</v>
-      </c>
-      <c r="C3" s="27">
-        <v>2074326.9500000002</v>
+        <v>24</v>
+      </c>
+      <c r="C3" s="27" cm="1">
+        <f t="array" ref="C3:C14">SUMIFS(staff[Salary],staff[Department],A3:A14)</f>
+        <v>2013215.1600000001</v>
       </c>
       <c r="D3" s="27">
         <f>AVERAGEIFS(staff[Salary],staff[Department],A3)</f>
-        <v>79781.805769230778</v>
+        <v>83883.965000000011</v>
       </c>
       <c r="E3">
         <f>COUNTIFS(staff[Employee type],"Permanent",staff[Department],A3)</f>
-        <v>18</v>
-      </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>11</v>
+      </c>
+      <c r="F3" cm="1">
+        <f t="array" ref="F3:F14">COUNTIFS(staff[Employee type],"Temporary",staff[Department],A3:A14)</f>
+        <v>7</v>
+      </c>
+      <c r="G3" cm="1">
+        <f t="array" ref="G3:G14">COUNTIFS(staff[Employee type],"Fixed Term",staff[Department],A3:A14)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <f>COUNTIF(staff[Department],A4)</f>
         <v>26</v>
       </c>
       <c r="C4" s="27">
-        <v>2131387.4899999998</v>
+        <v>2074326.9500000002</v>
       </c>
       <c r="D4" s="27">
         <f>AVERAGEIFS(staff[Salary],staff[Department],A4)</f>
-        <v>81976.441923076913</v>
+        <v>79781.805769230778</v>
       </c>
       <c r="E4">
         <f>COUNTIFS(staff[Employee type],"Permanent",staff[Department],A4)</f>
+        <v>18</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" t="s">
         <v>16</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>54</v>
       </c>
       <c r="B5">
         <f>COUNTIF(staff[Department],A5)</f>
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C5" s="27">
-        <v>773295.6</v>
+        <v>2131387.4899999998</v>
       </c>
       <c r="D5" s="27">
         <f>AVERAGEIFS(staff[Salary],staff[Department],A5)</f>
-        <v>64441.299999999996</v>
+        <v>81976.441923076913</v>
       </c>
       <c r="E5">
         <f>COUNTIFS(staff[Employee type],"Permanent",staff[Department],A5)</f>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>54</v>
       </c>
       <c r="B6">
         <f>COUNTIF(staff[Department],A6)</f>
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C6" s="27">
-        <v>1412092.87</v>
+        <v>773295.6</v>
       </c>
       <c r="D6" s="27">
         <f>AVERAGEIFS(staff[Salary],staff[Department],A6)</f>
-        <v>67242.51761904762</v>
+        <v>64441.299999999996</v>
       </c>
       <c r="E6">
         <f>COUNTIFS(staff[Employee type],"Permanent",staff[Department],A6)</f>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>131</v>
       </c>
       <c r="B7">
         <f>COUNTIF(staff[Department],A7)</f>
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C7" s="27">
-        <v>1814980.59</v>
+        <v>1412092.87</v>
       </c>
       <c r="D7" s="27">
         <f>AVERAGEIFS(staff[Salary],staff[Department],A7)</f>
-        <v>69806.945769230777</v>
+        <v>67242.51761904762</v>
       </c>
       <c r="E7">
         <f>COUNTIFS(staff[Employee type],"Permanent",staff[Department],A7)</f>
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B8">
         <f>COUNTIF(staff[Department],A8)</f>
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C8" s="27">
-        <v>1608406.3100000003</v>
+        <v>1814980.59</v>
       </c>
       <c r="D8" s="27">
         <f>AVERAGEIFS(staff[Salary],staff[Department],A8)</f>
-        <v>73109.377727272746</v>
+        <v>69806.945769230777</v>
       </c>
       <c r="E8">
         <f>COUNTIFS(staff[Employee type],"Permanent",staff[Department],A8)</f>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
       <c r="B9">
         <f>COUNTIF(staff[Department],A9)</f>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C9" s="27">
-        <v>1204393.78</v>
+        <v>1608406.3100000003</v>
       </c>
       <c r="D9" s="27">
         <f>AVERAGEIFS(staff[Salary],staff[Department],A9)</f>
-        <v>66910.765555555554</v>
+        <v>73109.377727272746</v>
       </c>
       <c r="E9">
         <f>COUNTIFS(staff[Employee type],"Permanent",staff[Department],A9)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F9">
         <v>3</v>
       </c>
       <c r="G9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="B10">
         <f>COUNTIF(staff[Department],A10)</f>
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C10" s="27">
-        <v>1568153.47</v>
+        <v>1204393.78</v>
       </c>
       <c r="D10" s="27">
         <f>AVERAGEIFS(staff[Salary],staff[Department],A10)</f>
-        <v>74673.974761904756</v>
+        <v>66910.765555555554</v>
       </c>
       <c r="E10">
         <f>COUNTIFS(staff[Employee type],"Permanent",staff[Department],A10)</f>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>32</v>
       </c>
       <c r="B11">
         <f>COUNTIF(staff[Department],A11)</f>
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C11" s="27">
-        <v>2180192.8699999992</v>
+        <v>1568153.47</v>
       </c>
       <c r="D11" s="27">
         <f>AVERAGEIFS(staff[Salary],staff[Department],A11)</f>
-        <v>75179.064482758593</v>
+        <v>74673.974761904756</v>
       </c>
       <c r="E11">
         <f>COUNTIFS(staff[Employee type],"Permanent",staff[Department],A11)</f>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
         <v>3</v>
       </c>
-      <c r="G11">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>124</v>
       </c>
       <c r="B12">
         <f>COUNTIF(staff[Department],A12)</f>
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C12" s="27">
-        <v>1129351.75</v>
+        <v>2180192.8699999992</v>
       </c>
       <c r="D12" s="27">
         <f>AVERAGEIFS(staff[Salary],staff[Department],A12)</f>
-        <v>66432.455882352937</v>
+        <v>75179.064482758593</v>
       </c>
       <c r="E12">
         <f>COUNTIFS(staff[Employee type],"Permanent",staff[Department],A12)</f>
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F12">
         <v>3</v>
       </c>
       <c r="G12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="B13">
         <f>COUNTIF(staff[Department],A13)</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="27">
-        <v>1294147.72</v>
+        <v>1129351.75</v>
       </c>
       <c r="D13" s="27">
         <f>AVERAGEIFS(staff[Salary],staff[Department],A13)</f>
-        <v>71897.095555555556</v>
+        <v>66432.455882352937</v>
       </c>
       <c r="E13">
         <f>COUNTIFS(staff[Employee type],"Permanent",staff[Department],A13)</f>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G13">
         <v>3</v>
       </c>
     </row>
+    <row r="14" spans="1:17">
+      <c r="A14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14">
+        <f>COUNTIF(staff[Department],A14)</f>
+        <v>18</v>
+      </c>
+      <c r="C14" s="27">
+        <v>1294147.72</v>
+      </c>
+      <c r="D14" s="27">
+        <f>AVERAGEIFS(staff[Salary],staff[Department],A14)</f>
+        <v>71897.095555555556</v>
+      </c>
+      <c r="E14">
+        <f>COUNTIFS(staff[Employee type],"Permanent",staff[Department],A14)</f>
+        <v>13</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="28.8">
+      <c r="A16" s="33" t="s">
+        <v>774</v>
+      </c>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+    </row>
+    <row r="17" spans="1:14" ht="14.4" customHeight="1">
+      <c r="A17" s="37" t="str" cm="1">
+        <f t="array" ref="A17:M17">staff[#Headers]</f>
+        <v>Emp ID</v>
+      </c>
+      <c r="B17" s="37" t="str">
+        <v>First Name</v>
+      </c>
+      <c r="C17" s="37" t="str">
+        <v>Last Name</v>
+      </c>
+      <c r="D17" s="37" t="str">
+        <v>Gender</v>
+      </c>
+      <c r="E17" s="37" t="str">
+        <v>Department</v>
+      </c>
+      <c r="F17" s="37" t="str">
+        <v>Salary</v>
+      </c>
+      <c r="G17" s="37" t="str">
+        <v>Salary Bucket</v>
+      </c>
+      <c r="H17" s="37" t="str">
+        <v>Start Date</v>
+      </c>
+      <c r="I17" s="37" t="str">
+        <v>FTE</v>
+      </c>
+      <c r="J17" s="37" t="str">
+        <v>Employee type</v>
+      </c>
+      <c r="K17" s="37" t="str">
+        <v>Work location</v>
+      </c>
+      <c r="L17" s="37" t="str">
+        <v>Tenure</v>
+      </c>
+      <c r="M17" s="37" t="str">
+        <v>Work Type</v>
+      </c>
+      <c r="N17" s="38"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" t="str" cm="1">
+        <f t="array" ref="A18:M64">_xlfn._xlws.FILTER(staff[],staff[Salary]&gt;=100000)</f>
+        <v>PR00147</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Minerva</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Ricardot</v>
+      </c>
+      <c r="D18" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E18" t="str">
+        <v>Engineering</v>
+      </c>
+      <c r="F18">
+        <v>120000</v>
+      </c>
+      <c r="G18" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H18" s="36">
+        <v>43416</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K18" t="str">
+        <v>Remote</v>
+      </c>
+      <c r="L18">
+        <v>5.6109589041095891</v>
+      </c>
+      <c r="M18" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" t="str">
+        <v>PR00746</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Hogan</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Iles</v>
+      </c>
+      <c r="D19" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E19" t="str">
+        <v>Accounting</v>
+      </c>
+      <c r="F19">
+        <v>114177.23</v>
+      </c>
+      <c r="G19" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H19" s="36">
+        <v>43908</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K19" t="str">
+        <v>Wellington, New Zealand</v>
+      </c>
+      <c r="L19">
+        <v>4.2630136986301368</v>
+      </c>
+      <c r="M19" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" t="str">
+        <v>PR01159</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Mollie</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Hanway</v>
+      </c>
+      <c r="D20" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E20" t="str">
+        <v>Engineering</v>
+      </c>
+      <c r="F20">
+        <v>112645.99</v>
+      </c>
+      <c r="G20" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H20" s="36">
+        <v>43759</v>
+      </c>
+      <c r="I20">
+        <v>0.6</v>
+      </c>
+      <c r="J20" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K20" t="str">
+        <v>Seattle, USA</v>
+      </c>
+      <c r="L20">
+        <v>4.6712328767123283</v>
+      </c>
+      <c r="M20" t="str">
+        <v>Part time</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" t="str">
+        <v>PR02010</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Prerana</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Nishita</v>
+      </c>
+      <c r="D21" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E21" t="str">
+        <v>Product Management</v>
+      </c>
+      <c r="F21">
+        <v>115191.38</v>
+      </c>
+      <c r="G21" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H21" s="36">
+        <v>44004</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K21" t="str">
+        <v>Hyderabad, India</v>
+      </c>
+      <c r="L21">
+        <v>4</v>
+      </c>
+      <c r="M21" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" t="str">
+        <v>PR02208</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Gowri</v>
+      </c>
+      <c r="C22" t="str">
+        <v>Sankar</v>
+      </c>
+      <c r="D22" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E22" t="str">
+        <v>Training</v>
+      </c>
+      <c r="F22">
+        <v>102934.09</v>
+      </c>
+      <c r="G22" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H22" s="36">
+        <v>44315</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K22" t="str">
+        <v>Hyderabad, India</v>
+      </c>
+      <c r="L22">
+        <v>3.1479452054794521</v>
+      </c>
+      <c r="M22" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" t="str">
+        <v>PR02288</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Althea</v>
+      </c>
+      <c r="C23" t="str">
+        <v>Bronger</v>
+      </c>
+      <c r="D23" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E23" t="str">
+        <v>Product Management</v>
+      </c>
+      <c r="F23">
+        <v>104335.03999999999</v>
+      </c>
+      <c r="G23" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H23" s="36">
+        <v>43874</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K23" t="str">
+        <v>Columbus, USA</v>
+      </c>
+      <c r="L23">
+        <v>4.3561643835616435</v>
+      </c>
+      <c r="M23" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" t="str">
+        <v>PR03886</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Edd</v>
+      </c>
+      <c r="C24" t="str">
+        <v>MacKnockiter</v>
+      </c>
+      <c r="D24" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E24" t="str">
+        <v>Accounting</v>
+      </c>
+      <c r="F24">
+        <v>119022.49</v>
+      </c>
+      <c r="G24" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H24" s="36">
+        <v>44431</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K24" t="str">
+        <v>Auckland, New Zealand</v>
+      </c>
+      <c r="L24">
+        <v>2.8301369863013699</v>
+      </c>
+      <c r="M24" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" t="str">
+        <v>PR04601</v>
+      </c>
+      <c r="B25" t="str">
+        <v>Yedukondalu</v>
+      </c>
+      <c r="C25" t="str">
+        <v>Panditula</v>
+      </c>
+      <c r="D25" t="str">
+        <v>Need to check</v>
+      </c>
+      <c r="E25" t="str">
+        <v>Support</v>
+      </c>
+      <c r="F25">
+        <v>104802.63</v>
+      </c>
+      <c r="G25" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H25" s="36">
+        <v>44502</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K25" t="str">
+        <v>Hyderabad, India</v>
+      </c>
+      <c r="L25">
+        <v>2.6356164383561644</v>
+      </c>
+      <c r="M25" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" t="str">
+        <v>SQ00022</v>
+      </c>
+      <c r="B26" t="str">
+        <v>Carlin</v>
+      </c>
+      <c r="C26" t="str">
+        <v>Demke</v>
+      </c>
+      <c r="D26" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E26" t="str">
+        <v>Business Development</v>
+      </c>
+      <c r="F26">
+        <v>110042.37</v>
+      </c>
+      <c r="G26" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H26" s="36">
+        <v>43914</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K26" t="str">
+        <v>Columbus, USA</v>
+      </c>
+      <c r="L26">
+        <v>4.2465753424657535</v>
+      </c>
+      <c r="M26" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" t="str">
+        <v>SQ00144</v>
+      </c>
+      <c r="B27" t="str">
+        <v>Collen</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Dunbleton</v>
+      </c>
+      <c r="D27" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E27" t="str">
+        <v>Engineering</v>
+      </c>
+      <c r="F27">
+        <v>118976.16</v>
+      </c>
+      <c r="G27" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H27" s="36">
+        <v>44120</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K27" t="str">
+        <v>Wellington, New Zealand</v>
+      </c>
+      <c r="L27">
+        <v>3.6821917808219178</v>
+      </c>
+      <c r="M27" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" t="str">
+        <v>SQ00498</v>
+      </c>
+      <c r="B28" t="str">
+        <v>Amery</v>
+      </c>
+      <c r="C28" t="str">
+        <v>Ofer</v>
+      </c>
+      <c r="D28" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E28" t="str">
+        <v>Legal</v>
+      </c>
+      <c r="F28">
+        <v>111049.84</v>
+      </c>
+      <c r="G28" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H28" s="36">
+        <v>44393</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K28" t="str">
+        <v>Wellington, New Zealand</v>
+      </c>
+      <c r="L28">
+        <v>2.9342465753424656</v>
+      </c>
+      <c r="M28" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" t="str">
+        <v>SQ01620</v>
+      </c>
+      <c r="B29" t="str">
+        <v>Westbrook</v>
+      </c>
+      <c r="C29" t="str">
+        <v>Brandino</v>
+      </c>
+      <c r="D29" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E29" t="str">
+        <v>Legal</v>
+      </c>
+      <c r="F29">
+        <v>113616.23</v>
+      </c>
+      <c r="G29" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H29" s="36">
+        <v>43255</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K29" t="str">
+        <v>Remote</v>
+      </c>
+      <c r="L29">
+        <v>6.0520547945205481</v>
+      </c>
+      <c r="M29" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" t="str">
+        <v>SQ02035</v>
+      </c>
+      <c r="B30" t="str">
+        <v>Anni</v>
+      </c>
+      <c r="C30" t="str">
+        <v>Izzard</v>
+      </c>
+      <c r="D30" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E30" t="str">
+        <v>Human Resources</v>
+      </c>
+      <c r="F30">
+        <v>103494.94</v>
+      </c>
+      <c r="G30" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H30" s="36">
+        <v>43256</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K30" t="str">
+        <v>Remote</v>
+      </c>
+      <c r="L30">
+        <v>6.0493150684931507</v>
+      </c>
+      <c r="M30" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" t="str">
+        <v>SQ02035</v>
+      </c>
+      <c r="B31" t="str">
+        <v>Anni</v>
+      </c>
+      <c r="C31" t="str">
+        <v>Izzard</v>
+      </c>
+      <c r="D31" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E31" t="str">
+        <v>Human Resources</v>
+      </c>
+      <c r="F31">
+        <v>103494.94</v>
+      </c>
+      <c r="G31" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H31" s="36">
+        <v>43256</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K31" t="str">
+        <v>Remote</v>
+      </c>
+      <c r="L31">
+        <v>6.0493150684931507</v>
+      </c>
+      <c r="M31" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" t="str">
+        <v>SQ02174</v>
+      </c>
+      <c r="B32" t="str">
+        <v>Sidoney</v>
+      </c>
+      <c r="C32" t="str">
+        <v>Yitzhok</v>
+      </c>
+      <c r="D32" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E32" t="str">
+        <v>Engineering</v>
+      </c>
+      <c r="F32">
+        <v>118442.54</v>
+      </c>
+      <c r="G32" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H32" s="36">
+        <v>44193</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K32" t="str">
+        <v>Auckland, New Zealand</v>
+      </c>
+      <c r="L32">
+        <v>3.4821917808219176</v>
+      </c>
+      <c r="M32" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" t="str">
+        <v>SQ02624</v>
+      </c>
+      <c r="B33" t="str">
+        <v>Gwenneth</v>
+      </c>
+      <c r="C33" t="str">
+        <v>Fealey</v>
+      </c>
+      <c r="D33" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E33" t="str">
+        <v>Engineering</v>
+      </c>
+      <c r="F33">
+        <v>114772.32</v>
+      </c>
+      <c r="G33" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H33" s="36">
+        <v>44251</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K33" t="str">
+        <v>Columbus, USA</v>
+      </c>
+      <c r="L33">
+        <v>3.3232876712328765</v>
+      </c>
+      <c r="M33" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" t="str">
+        <v>SQ02703</v>
+      </c>
+      <c r="B34" t="str">
+        <v>Deepit</v>
+      </c>
+      <c r="C34" t="str">
+        <v>Ranjana</v>
+      </c>
+      <c r="D34" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E34" t="str">
+        <v>Marketing</v>
+      </c>
+      <c r="F34">
+        <v>104903.79</v>
+      </c>
+      <c r="G34" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H34" s="36">
+        <v>43649</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K34" t="str">
+        <v>Chennai, India</v>
+      </c>
+      <c r="L34">
+        <v>4.9726027397260273</v>
+      </c>
+      <c r="M34" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" t="str">
+        <v>SQ03116</v>
+      </c>
+      <c r="B35" t="str">
+        <v>Syd</v>
+      </c>
+      <c r="C35" t="str">
+        <v>Fearn</v>
+      </c>
+      <c r="D35" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E35" t="str">
+        <v>Engineering</v>
+      </c>
+      <c r="F35">
+        <v>108872.77</v>
+      </c>
+      <c r="G35" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H35" s="36">
+        <v>43521</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K35" t="str">
+        <v>Remote</v>
+      </c>
+      <c r="L35">
+        <v>5.3232876712328769</v>
+      </c>
+      <c r="M35" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" t="str">
+        <v>SQ03387</v>
+      </c>
+      <c r="B36" t="str">
+        <v>Robinia</v>
+      </c>
+      <c r="C36" t="str">
+        <v>Scholling</v>
+      </c>
+      <c r="D36" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E36" t="str">
+        <v>Human Resources</v>
+      </c>
+      <c r="F36">
+        <v>100731.95</v>
+      </c>
+      <c r="G36" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H36" s="36">
+        <v>43936</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K36" t="str">
+        <v>Auckland, New Zealand</v>
+      </c>
+      <c r="L36">
+        <v>4.1863013698630134</v>
+      </c>
+      <c r="M36" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" t="str">
+        <v>SQ03476</v>
+      </c>
+      <c r="B37" t="str">
+        <v>Ramalingam</v>
+      </c>
+      <c r="C37" t="str">
+        <v>Kothapeta</v>
+      </c>
+      <c r="D37" t="str">
+        <v>Need to check</v>
+      </c>
+      <c r="E37" t="str">
+        <v>Accounting</v>
+      </c>
+      <c r="F37">
+        <v>107107.6</v>
+      </c>
+      <c r="G37" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H37" s="36">
+        <v>43325</v>
+      </c>
+      <c r="I37">
+        <v>0.9</v>
+      </c>
+      <c r="J37" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K37" t="str">
+        <v>Chennai, India</v>
+      </c>
+      <c r="L37">
+        <v>5.86027397260274</v>
+      </c>
+      <c r="M37" t="str">
+        <v>Part time</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" t="str">
+        <v>SQ03491</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Freda</v>
+      </c>
+      <c r="C38" t="str">
+        <v>Legan</v>
+      </c>
+      <c r="D38" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E38" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="F38">
+        <v>102129.37</v>
+      </c>
+      <c r="G38" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H38" s="36">
+        <v>44396</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K38" t="str">
+        <v>Columbus, USA</v>
+      </c>
+      <c r="L38">
+        <v>2.9260273972602739</v>
+      </c>
+      <c r="M38" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" t="str">
+        <v>SQ03733</v>
+      </c>
+      <c r="B39" t="str">
+        <v>Revkah</v>
+      </c>
+      <c r="C39" t="str">
+        <v>Antonacci</v>
+      </c>
+      <c r="D39" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E39" t="str">
+        <v>Engineering</v>
+      </c>
+      <c r="F39">
+        <v>109143.17</v>
+      </c>
+      <c r="G39" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H39" s="36">
+        <v>43945</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K39" t="str">
+        <v>Wellington, New Zealand</v>
+      </c>
+      <c r="L39">
+        <v>4.161643835616438</v>
+      </c>
+      <c r="M39" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" t="str">
+        <v>SQ04603</v>
+      </c>
+      <c r="B40" t="str">
+        <v>Natalee</v>
+      </c>
+      <c r="C40" t="str">
+        <v>Craiker</v>
+      </c>
+      <c r="D40" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E40" t="str">
+        <v>Product Management</v>
+      </c>
+      <c r="F40">
+        <v>111229.47</v>
+      </c>
+      <c r="G40" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H40" s="36">
+        <v>43402</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K40" t="str">
+        <v>Remote</v>
+      </c>
+      <c r="L40">
+        <v>5.6493150684931503</v>
+      </c>
+      <c r="M40" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" t="str">
+        <v>SQ04612</v>
+      </c>
+      <c r="B41" t="str">
+        <v>Mick</v>
+      </c>
+      <c r="C41" t="str">
+        <v>Spraberry</v>
+      </c>
+      <c r="D41" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E41" t="str">
+        <v>Services</v>
+      </c>
+      <c r="F41">
+        <v>120000</v>
+      </c>
+      <c r="G41" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H41" s="36">
+        <v>43902</v>
+      </c>
+      <c r="I41">
+        <v>0.9</v>
+      </c>
+      <c r="J41" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K41" t="str">
+        <v>Remote</v>
+      </c>
+      <c r="L41">
+        <v>4.279452054794521</v>
+      </c>
+      <c r="M41" t="str">
+        <v>Part time</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" t="str">
+        <v>SQ04665</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Collin</v>
+      </c>
+      <c r="C42" t="str">
+        <v>Jagson</v>
+      </c>
+      <c r="D42" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E42" t="str">
+        <v>Services</v>
+      </c>
+      <c r="F42">
+        <v>100424.23</v>
+      </c>
+      <c r="G42" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H42" s="36">
+        <v>43801</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="J42" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K42" t="str">
+        <v>Auckland, New Zealand</v>
+      </c>
+      <c r="L42">
+        <v>4.5561643835616437</v>
+      </c>
+      <c r="M42" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" t="str">
+        <v>TN00579</v>
+      </c>
+      <c r="B43" t="str">
+        <v>Rafaelita</v>
+      </c>
+      <c r="C43" t="str">
+        <v>Blaksland</v>
+      </c>
+      <c r="D43" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E43" t="str">
+        <v>Services</v>
+      </c>
+      <c r="F43">
+        <v>109163.39</v>
+      </c>
+      <c r="G43" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H43" s="36">
+        <v>44019</v>
+      </c>
+      <c r="I43">
+        <v>0.8</v>
+      </c>
+      <c r="J43" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K43" t="str">
+        <v>Seattle, USA</v>
+      </c>
+      <c r="L43">
+        <v>3.9589041095890409</v>
+      </c>
+      <c r="M43" t="str">
+        <v>Part time</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" t="str">
+        <v>TN01281</v>
+      </c>
+      <c r="B44" t="str">
+        <v>Cletus</v>
+      </c>
+      <c r="C44" t="str">
+        <v>McGarahan</v>
+      </c>
+      <c r="D44" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E44" t="str">
+        <v>Engineering</v>
+      </c>
+      <c r="F44">
+        <v>114425.19</v>
+      </c>
+      <c r="G44" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H44" s="36">
+        <v>43857</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K44" t="str">
+        <v>Wellington, New Zealand</v>
+      </c>
+      <c r="L44">
+        <v>4.4027397260273968</v>
+      </c>
+      <c r="M44" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" t="str">
+        <v>TN04058</v>
+      </c>
+      <c r="B45" t="str">
+        <v>Subbarao</v>
+      </c>
+      <c r="C45" t="str">
+        <v>Malladi</v>
+      </c>
+      <c r="D45" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E45" t="str">
+        <v>Product Management</v>
+      </c>
+      <c r="F45">
+        <v>106775.14</v>
+      </c>
+      <c r="G45" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H45" s="36">
+        <v>43563</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="J45" t="str">
+        <v>Fixed Term</v>
+      </c>
+      <c r="K45" t="str">
+        <v>Hyderabad, India</v>
+      </c>
+      <c r="L45">
+        <v>5.2082191780821914</v>
+      </c>
+      <c r="M45" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" t="str">
+        <v>TN04058</v>
+      </c>
+      <c r="B46" t="str">
+        <v>Vasu</v>
+      </c>
+      <c r="C46" t="str">
+        <v>Nandin</v>
+      </c>
+      <c r="D46" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E46" t="str">
+        <v>Product Management</v>
+      </c>
+      <c r="F46">
+        <v>106775.14</v>
+      </c>
+      <c r="G46" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H46" s="36">
+        <v>43563</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="J46" t="str">
+        <v>Fixed Term</v>
+      </c>
+      <c r="K46" t="str">
+        <v>Hyderabad, India</v>
+      </c>
+      <c r="L46">
+        <v>5.2082191780821914</v>
+      </c>
+      <c r="M46" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" t="str">
+        <v>TN04246</v>
+      </c>
+      <c r="B47" t="str">
+        <v>Shaylyn</v>
+      </c>
+      <c r="C47" t="str">
+        <v>Ransbury</v>
+      </c>
+      <c r="D47" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E47" t="str">
+        <v>Support</v>
+      </c>
+      <c r="F47">
+        <v>100371.31</v>
+      </c>
+      <c r="G47" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H47" s="36">
+        <v>44067</v>
+      </c>
+      <c r="I47">
+        <v>0.8</v>
+      </c>
+      <c r="J47" t="str">
+        <v>Fixed Term</v>
+      </c>
+      <c r="K47" t="str">
+        <v>Auckland, New Zealand</v>
+      </c>
+      <c r="L47">
+        <v>3.8273972602739725</v>
+      </c>
+      <c r="M47" t="str">
+        <v>Part time</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" t="str">
+        <v>TN04740</v>
+      </c>
+      <c r="B48" t="str">
+        <v>Tristam</v>
+      </c>
+      <c r="C48" t="str">
+        <v>Cuming</v>
+      </c>
+      <c r="D48" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E48" t="str">
+        <v>Support</v>
+      </c>
+      <c r="F48">
+        <v>104038.9</v>
+      </c>
+      <c r="G48" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H48" s="36">
+        <v>43815</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48" t="str">
+        <v>Fixed Term</v>
+      </c>
+      <c r="K48" t="str">
+        <v>Remote</v>
+      </c>
+      <c r="L48">
+        <v>4.5178082191780824</v>
+      </c>
+      <c r="M48" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" t="str">
+        <v>VT01684</v>
+      </c>
+      <c r="B49" t="str">
+        <v>Audry</v>
+      </c>
+      <c r="C49" t="str">
+        <v>Yu</v>
+      </c>
+      <c r="D49" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E49" t="str">
+        <v>Training</v>
+      </c>
+      <c r="F49">
+        <v>101187.36</v>
+      </c>
+      <c r="G49" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H49" s="36">
+        <v>43258</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="J49" t="str">
+        <v>Fixed Term</v>
+      </c>
+      <c r="K49" t="str">
+        <v>Columbus, USA</v>
+      </c>
+      <c r="L49">
+        <v>6.043835616438356</v>
+      </c>
+      <c r="M49" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" t="str">
+        <v>VT01762</v>
+      </c>
+      <c r="B50" t="str">
+        <v>Geena</v>
+      </c>
+      <c r="C50" t="str">
+        <v>Raghavanpillai</v>
+      </c>
+      <c r="D50" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E50" t="str">
+        <v>Accounting</v>
+      </c>
+      <c r="F50">
+        <v>102515.81</v>
+      </c>
+      <c r="G50" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H50" s="36">
+        <v>43902</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50" t="str">
+        <v>Fixed Term</v>
+      </c>
+      <c r="K50" t="str">
+        <v>Chennai, India</v>
+      </c>
+      <c r="L50">
+        <v>4.279452054794521</v>
+      </c>
+      <c r="M50" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" t="str">
+        <v>VT01893</v>
+      </c>
+      <c r="B51" t="str">
+        <v>Lindy</v>
+      </c>
+      <c r="C51" t="str">
+        <v>Guillet</v>
+      </c>
+      <c r="D51" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E51" t="str">
+        <v>Training</v>
+      </c>
+      <c r="F51">
+        <v>112778.28</v>
+      </c>
+      <c r="G51" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H51" s="36">
+        <v>43250</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51" t="str">
+        <v>Fixed Term</v>
+      </c>
+      <c r="K51" t="str">
+        <v>Remote</v>
+      </c>
+      <c r="L51">
+        <v>6.065753424657534</v>
+      </c>
+      <c r="M51" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" t="str">
+        <v>VT01893</v>
+      </c>
+      <c r="B52" t="str">
+        <v>Lindy</v>
+      </c>
+      <c r="C52" t="str">
+        <v>Guillet</v>
+      </c>
+      <c r="D52" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E52" t="str">
+        <v>Training</v>
+      </c>
+      <c r="F52">
+        <v>112778.28</v>
+      </c>
+      <c r="G52" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H52" s="36">
+        <v>43250</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="J52" t="str">
+        <v>Fixed Term</v>
+      </c>
+      <c r="K52" t="str">
+        <v>Remote</v>
+      </c>
+      <c r="L52">
+        <v>6.065753424657534</v>
+      </c>
+      <c r="M52" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" t="str">
+        <v>VT02491</v>
+      </c>
+      <c r="B53" t="str">
+        <v>Alexis</v>
+      </c>
+      <c r="C53" t="str">
+        <v>Gotfrey</v>
+      </c>
+      <c r="D53" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E53" t="str">
+        <v>Engineering</v>
+      </c>
+      <c r="F53">
+        <v>114465.93</v>
+      </c>
+      <c r="G53" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H53" s="36">
+        <v>43291</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53" t="str">
+        <v>Temporary</v>
+      </c>
+      <c r="K53" t="str">
+        <v>Wellington, New Zealand</v>
+      </c>
+      <c r="L53">
+        <v>5.9534246575342467</v>
+      </c>
+      <c r="M53" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" t="str">
+        <v>VT02801</v>
+      </c>
+      <c r="B54" t="str">
+        <v>Shellysheldon</v>
+      </c>
+      <c r="C54" t="str">
+        <v>Mahady</v>
+      </c>
+      <c r="D54" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E54" t="str">
+        <v>Training</v>
+      </c>
+      <c r="F54">
+        <v>114691.03</v>
+      </c>
+      <c r="G54" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H54" s="36">
+        <v>44039</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="J54" t="str">
+        <v>Temporary</v>
+      </c>
+      <c r="K54" t="str">
+        <v>Wellington, New Zealand</v>
+      </c>
+      <c r="L54">
+        <v>3.904109589041096</v>
+      </c>
+      <c r="M54" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" t="str">
+        <v>VT03421</v>
+      </c>
+      <c r="B55" t="str">
+        <v>Alic</v>
+      </c>
+      <c r="C55" t="str">
+        <v>Bagg</v>
+      </c>
+      <c r="D55" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E55" t="str">
+        <v>Legal</v>
+      </c>
+      <c r="F55">
+        <v>113747.56</v>
+      </c>
+      <c r="G55" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H55" s="36">
+        <v>44270</v>
+      </c>
+      <c r="I55">
+        <v>0.7</v>
+      </c>
+      <c r="J55" t="str">
+        <v>Temporary</v>
+      </c>
+      <c r="K55" t="str">
+        <v>Columbus, USA</v>
+      </c>
+      <c r="L55">
+        <v>3.2712328767123289</v>
+      </c>
+      <c r="M55" t="str">
+        <v>Part time</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56" t="str">
+        <v>VT03421</v>
+      </c>
+      <c r="B56" t="str">
+        <v>Alic</v>
+      </c>
+      <c r="C56" t="str">
+        <v>Bagg</v>
+      </c>
+      <c r="D56" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E56" t="str">
+        <v>Legal</v>
+      </c>
+      <c r="F56">
+        <v>113747.56</v>
+      </c>
+      <c r="G56" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H56" s="36">
+        <v>44270</v>
+      </c>
+      <c r="I56">
+        <v>0.7</v>
+      </c>
+      <c r="J56" t="str">
+        <v>Temporary</v>
+      </c>
+      <c r="K56" t="str">
+        <v>Columbus, USA</v>
+      </c>
+      <c r="L56">
+        <v>3.2712328767123289</v>
+      </c>
+      <c r="M56" t="str">
+        <v>Part time</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57" t="str">
+        <v>VT04028</v>
+      </c>
+      <c r="B57" t="str">
+        <v>Michale</v>
+      </c>
+      <c r="C57" t="str">
+        <v>Rolf</v>
+      </c>
+      <c r="D57" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E57" t="str">
+        <v>Services</v>
+      </c>
+      <c r="F57">
+        <v>111815.49</v>
+      </c>
+      <c r="G57" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H57" s="36">
+        <v>43895</v>
+      </c>
+      <c r="I57">
+        <v>0.7</v>
+      </c>
+      <c r="J57" t="str">
+        <v>Temporary</v>
+      </c>
+      <c r="K57" t="str">
+        <v>Remote</v>
+      </c>
+      <c r="L57">
+        <v>4.2986301369863016</v>
+      </c>
+      <c r="M57" t="str">
+        <v>Part time</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
+      <c r="A58" t="str">
+        <v>VT04028</v>
+      </c>
+      <c r="B58" t="str">
+        <v>Michale</v>
+      </c>
+      <c r="C58" t="str">
+        <v>Rolf</v>
+      </c>
+      <c r="D58" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E58" t="str">
+        <v>Services</v>
+      </c>
+      <c r="F58">
+        <v>111815.49</v>
+      </c>
+      <c r="G58" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H58" s="36">
+        <v>43895</v>
+      </c>
+      <c r="I58">
+        <v>0.7</v>
+      </c>
+      <c r="J58" t="str">
+        <v>Temporary</v>
+      </c>
+      <c r="K58" t="str">
+        <v>Remote</v>
+      </c>
+      <c r="L58">
+        <v>4.2986301369863016</v>
+      </c>
+      <c r="M58" t="str">
+        <v>Part time</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
+      <c r="A59" t="str">
+        <v>VT04093</v>
+      </c>
+      <c r="B59" t="str">
+        <v>Prasanna</v>
+      </c>
+      <c r="C59" t="str">
+        <v>Lakshmi</v>
+      </c>
+      <c r="D59" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E59" t="str">
+        <v>Training</v>
+      </c>
+      <c r="F59">
+        <v>116767.63</v>
+      </c>
+      <c r="G59" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H59" s="36">
+        <v>43949</v>
+      </c>
+      <c r="I59">
+        <v>0.4</v>
+      </c>
+      <c r="J59" t="str">
+        <v>Temporary</v>
+      </c>
+      <c r="K59" t="str">
+        <v>Chennai, India</v>
+      </c>
+      <c r="L59">
+        <v>4.1506849315068495</v>
+      </c>
+      <c r="M59" t="str">
+        <v>Part time</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="A60" t="str">
+        <v>VT04093</v>
+      </c>
+      <c r="B60" t="str">
+        <v>Baruna</v>
+      </c>
+      <c r="C60" t="str">
+        <v>Ogale</v>
+      </c>
+      <c r="D60" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E60" t="str">
+        <v>Training</v>
+      </c>
+      <c r="F60">
+        <v>116767.63</v>
+      </c>
+      <c r="G60" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H60" s="36">
+        <v>43949</v>
+      </c>
+      <c r="I60">
+        <v>0.4</v>
+      </c>
+      <c r="J60" t="str">
+        <v>Temporary</v>
+      </c>
+      <c r="K60" t="str">
+        <v>Chennai, India</v>
+      </c>
+      <c r="L60">
+        <v>4.1506849315068495</v>
+      </c>
+      <c r="M60" t="str">
+        <v>Part time</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="A61" t="str">
+        <v>VT04350</v>
+      </c>
+      <c r="B61" t="str">
+        <v>Kulbhushan</v>
+      </c>
+      <c r="C61" t="str">
+        <v>Moorthy</v>
+      </c>
+      <c r="D61" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E61" t="str">
+        <v>Business Development</v>
+      </c>
+      <c r="F61">
+        <v>106400.02</v>
+      </c>
+      <c r="G61" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H61" s="36">
+        <v>44021</v>
+      </c>
+      <c r="I61">
+        <v>1</v>
+      </c>
+      <c r="J61" t="str">
+        <v>Temporary</v>
+      </c>
+      <c r="K61" t="str">
+        <v>Chennai, India</v>
+      </c>
+      <c r="L61">
+        <v>3.9534246575342467</v>
+      </c>
+      <c r="M61" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
+      <c r="A62" t="str">
+        <v>VT04350</v>
+      </c>
+      <c r="B62" t="str">
+        <v>Lalit</v>
+      </c>
+      <c r="C62" t="str">
+        <v>Kothari</v>
+      </c>
+      <c r="D62" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E62" t="str">
+        <v>Business Development</v>
+      </c>
+      <c r="F62">
+        <v>106400.02</v>
+      </c>
+      <c r="G62" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H62" s="36">
+        <v>44021</v>
+      </c>
+      <c r="I62">
+        <v>1</v>
+      </c>
+      <c r="J62" t="str">
+        <v>Temporary</v>
+      </c>
+      <c r="K62" t="str">
+        <v>Chennai, India</v>
+      </c>
+      <c r="L62">
+        <v>3.9534246575342467</v>
+      </c>
+      <c r="M62" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
+      <c r="A63" t="str">
+        <v>VT04552</v>
+      </c>
+      <c r="B63" t="str">
+        <v>Theresita</v>
+      </c>
+      <c r="C63" t="str">
+        <v>Chasmer</v>
+      </c>
+      <c r="D63" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E63" t="str">
+        <v>Product Management</v>
+      </c>
+      <c r="F63">
+        <v>106665.67</v>
+      </c>
+      <c r="G63" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H63" s="36">
+        <v>43311</v>
+      </c>
+      <c r="I63">
+        <v>1</v>
+      </c>
+      <c r="J63" t="str">
+        <v>Temporary</v>
+      </c>
+      <c r="K63" t="str">
+        <v>Columbus, USA</v>
+      </c>
+      <c r="L63">
+        <v>5.8986301369863012</v>
+      </c>
+      <c r="M63" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
+      <c r="A64" t="str">
+        <v>VT04681</v>
+      </c>
+      <c r="B64" t="str">
+        <v>Nickolai</v>
+      </c>
+      <c r="C64" t="str">
+        <v>Artin</v>
+      </c>
+      <c r="D64" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E64" t="str">
+        <v>Product Management</v>
+      </c>
+      <c r="F64">
+        <v>110906.35</v>
+      </c>
+      <c r="G64" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H64" s="36">
+        <v>43434</v>
+      </c>
+      <c r="I64">
+        <v>1</v>
+      </c>
+      <c r="J64" t="str">
+        <v>Temporary</v>
+      </c>
+      <c r="K64" t="str">
+        <v>Wellington, New Zealand</v>
+      </c>
+      <c r="L64">
+        <v>5.5616438356164384</v>
+      </c>
+      <c r="M64" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
+      <c r="H65" s="36"/>
+    </row>
+    <row r="66" spans="1:13" ht="18">
+      <c r="A66" s="29" t="s">
+        <v>776</v>
+      </c>
+      <c r="B66" s="29"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="29"/>
+      <c r="E66" s="29"/>
+      <c r="F66" s="29"/>
+      <c r="G66" s="29"/>
+      <c r="H66" s="45" t="s">
+        <v>777</v>
+      </c>
+      <c r="I66" s="45"/>
+      <c r="J66" s="45"/>
+    </row>
+    <row r="67" spans="1:13">
+      <c r="B67" s="28" t="s">
+        <v>775</v>
+      </c>
+      <c r="C67" s="28"/>
+      <c r="D67" s="28"/>
+      <c r="E67" s="28"/>
+      <c r="F67" s="44">
+        <v>115000</v>
+      </c>
+      <c r="H67" s="36"/>
+    </row>
+    <row r="68" spans="1:13">
+      <c r="A68" s="42" t="str" cm="1">
+        <f t="array" ref="A68:M68">staff[#Headers]</f>
+        <v>Emp ID</v>
+      </c>
+      <c r="B68" s="42" t="str">
+        <v>First Name</v>
+      </c>
+      <c r="C68" s="42" t="str">
+        <v>Last Name</v>
+      </c>
+      <c r="D68" s="42" t="str">
+        <v>Gender</v>
+      </c>
+      <c r="E68" s="42" t="str">
+        <v>Department</v>
+      </c>
+      <c r="F68" s="42" t="str">
+        <v>Salary</v>
+      </c>
+      <c r="G68" s="42" t="str">
+        <v>Salary Bucket</v>
+      </c>
+      <c r="H68" s="43" t="str">
+        <v>Start Date</v>
+      </c>
+      <c r="I68" s="42" t="str">
+        <v>FTE</v>
+      </c>
+      <c r="J68" s="42" t="str">
+        <v>Employee type</v>
+      </c>
+      <c r="K68" s="42" t="str">
+        <v>Work location</v>
+      </c>
+      <c r="L68" s="42" t="str">
+        <v>Tenure</v>
+      </c>
+      <c r="M68" s="42" t="str">
+        <v>Work Type</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13">
+      <c r="A69" s="36" t="str" cm="1">
+        <f t="array" ref="A69:M76">_xlfn._xlws.FILTER(staff[],staff[Salary]&gt;=F67)</f>
+        <v>PR00147</v>
+      </c>
+      <c r="B69" t="str">
+        <v>Minerva</v>
+      </c>
+      <c r="C69" t="str">
+        <v>Ricardot</v>
+      </c>
+      <c r="D69" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E69" t="str">
+        <v>Engineering</v>
+      </c>
+      <c r="F69">
+        <v>120000</v>
+      </c>
+      <c r="G69" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H69" s="36">
+        <v>43416</v>
+      </c>
+      <c r="I69">
+        <v>1</v>
+      </c>
+      <c r="J69" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K69" t="str">
+        <v>Remote</v>
+      </c>
+      <c r="L69">
+        <v>5.6109589041095891</v>
+      </c>
+      <c r="M69" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13">
+      <c r="A70" t="str">
+        <v>PR02010</v>
+      </c>
+      <c r="B70" t="str">
+        <v>Prerana</v>
+      </c>
+      <c r="C70" t="str">
+        <v>Nishita</v>
+      </c>
+      <c r="D70" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E70" t="str">
+        <v>Product Management</v>
+      </c>
+      <c r="F70">
+        <v>115191.38</v>
+      </c>
+      <c r="G70" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H70" s="36">
+        <v>44004</v>
+      </c>
+      <c r="I70">
+        <v>1</v>
+      </c>
+      <c r="J70" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K70" t="str">
+        <v>Hyderabad, India</v>
+      </c>
+      <c r="L70">
+        <v>4</v>
+      </c>
+      <c r="M70" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13">
+      <c r="A71" t="str">
+        <v>PR03886</v>
+      </c>
+      <c r="B71" t="str">
+        <v>Edd</v>
+      </c>
+      <c r="C71" t="str">
+        <v>MacKnockiter</v>
+      </c>
+      <c r="D71" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E71" t="str">
+        <v>Accounting</v>
+      </c>
+      <c r="F71">
+        <v>119022.49</v>
+      </c>
+      <c r="G71" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H71" s="36">
+        <v>44431</v>
+      </c>
+      <c r="I71">
+        <v>1</v>
+      </c>
+      <c r="J71" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K71" t="str">
+        <v>Auckland, New Zealand</v>
+      </c>
+      <c r="L71">
+        <v>2.8301369863013699</v>
+      </c>
+      <c r="M71" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13">
+      <c r="A72" t="str">
+        <v>SQ00144</v>
+      </c>
+      <c r="B72" t="str">
+        <v>Collen</v>
+      </c>
+      <c r="C72" t="str">
+        <v>Dunbleton</v>
+      </c>
+      <c r="D72" t="str">
+        <v>Male</v>
+      </c>
+      <c r="E72" t="str">
+        <v>Engineering</v>
+      </c>
+      <c r="F72">
+        <v>118976.16</v>
+      </c>
+      <c r="G72" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H72" s="36">
+        <v>44120</v>
+      </c>
+      <c r="I72">
+        <v>1</v>
+      </c>
+      <c r="J72" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K72" t="str">
+        <v>Wellington, New Zealand</v>
+      </c>
+      <c r="L72">
+        <v>3.6821917808219178</v>
+      </c>
+      <c r="M72" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13">
+      <c r="A73" t="str">
+        <v>SQ02174</v>
+      </c>
+      <c r="B73" t="str">
+        <v>Sidoney</v>
+      </c>
+      <c r="C73" t="str">
+        <v>Yitzhok</v>
+      </c>
+      <c r="D73" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E73" t="str">
+        <v>Engineering</v>
+      </c>
+      <c r="F73">
+        <v>118442.54</v>
+      </c>
+      <c r="G73" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H73" s="36">
+        <v>44193</v>
+      </c>
+      <c r="I73">
+        <v>1</v>
+      </c>
+      <c r="J73" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K73" t="str">
+        <v>Auckland, New Zealand</v>
+      </c>
+      <c r="L73">
+        <v>3.4821917808219176</v>
+      </c>
+      <c r="M73" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13">
+      <c r="A74" t="str">
+        <v>SQ04612</v>
+      </c>
+      <c r="B74" t="str">
+        <v>Mick</v>
+      </c>
+      <c r="C74" t="str">
+        <v>Spraberry</v>
+      </c>
+      <c r="D74" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E74" t="str">
+        <v>Services</v>
+      </c>
+      <c r="F74">
+        <v>120000</v>
+      </c>
+      <c r="G74" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H74" s="36">
+        <v>43902</v>
+      </c>
+      <c r="I74">
+        <v>0.9</v>
+      </c>
+      <c r="J74" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K74" t="str">
+        <v>Remote</v>
+      </c>
+      <c r="L74">
+        <v>4.279452054794521</v>
+      </c>
+      <c r="M74" t="str">
+        <v>Part time</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13">
+      <c r="A75" t="str">
+        <v>VT04093</v>
+      </c>
+      <c r="B75" t="str">
+        <v>Prasanna</v>
+      </c>
+      <c r="C75" t="str">
+        <v>Lakshmi</v>
+      </c>
+      <c r="D75" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E75" t="str">
+        <v>Training</v>
+      </c>
+      <c r="F75">
+        <v>116767.63</v>
+      </c>
+      <c r="G75" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H75" s="36">
+        <v>43949</v>
+      </c>
+      <c r="I75">
+        <v>0.4</v>
+      </c>
+      <c r="J75" t="str">
+        <v>Temporary</v>
+      </c>
+      <c r="K75" t="str">
+        <v>Chennai, India</v>
+      </c>
+      <c r="L75">
+        <v>4.1506849315068495</v>
+      </c>
+      <c r="M75" t="str">
+        <v>Part time</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13">
+      <c r="A76" t="str">
+        <v>VT04093</v>
+      </c>
+      <c r="B76" t="str">
+        <v>Baruna</v>
+      </c>
+      <c r="C76" t="str">
+        <v>Ogale</v>
+      </c>
+      <c r="D76" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E76" t="str">
+        <v>Training</v>
+      </c>
+      <c r="F76">
+        <v>116767.63</v>
+      </c>
+      <c r="G76" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H76" s="36">
+        <v>43949</v>
+      </c>
+      <c r="I76">
+        <v>0.4</v>
+      </c>
+      <c r="J76" t="str">
+        <v>Temporary</v>
+      </c>
+      <c r="K76" t="str">
+        <v>Chennai, India</v>
+      </c>
+      <c r="L76">
+        <v>4.1506849315068495</v>
+      </c>
+      <c r="M76" t="str">
+        <v>Part time</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13">
+      <c r="H77" s="36"/>
+    </row>
+    <row r="78" spans="1:13" ht="21">
+      <c r="A78" s="30" t="s">
+        <v>778</v>
+      </c>
+      <c r="B78" s="30"/>
+      <c r="C78" s="30"/>
+      <c r="D78" s="30"/>
+      <c r="E78" s="30"/>
+      <c r="F78" s="30"/>
+      <c r="G78" s="30"/>
+      <c r="H78" s="30"/>
+      <c r="I78" s="30"/>
+      <c r="J78" s="30"/>
+      <c r="K78" s="30"/>
+      <c r="L78" s="30"/>
+    </row>
+    <row r="79" spans="1:13">
+      <c r="A79" s="42" t="str" cm="1">
+        <f t="array" ref="A79:M79">staff[#Headers]</f>
+        <v>Emp ID</v>
+      </c>
+      <c r="B79" s="42" t="str">
+        <v>First Name</v>
+      </c>
+      <c r="C79" s="42" t="str">
+        <v>Last Name</v>
+      </c>
+      <c r="D79" s="42" t="str">
+        <v>Gender</v>
+      </c>
+      <c r="E79" s="42" t="str">
+        <v>Department</v>
+      </c>
+      <c r="F79" s="42" t="str">
+        <v>Salary</v>
+      </c>
+      <c r="G79" s="42" t="str">
+        <v>Salary Bucket</v>
+      </c>
+      <c r="H79" s="43" t="str">
+        <v>Start Date</v>
+      </c>
+      <c r="I79" s="42" t="str">
+        <v>FTE</v>
+      </c>
+      <c r="J79" s="42" t="str">
+        <v>Employee type</v>
+      </c>
+      <c r="K79" s="42" t="str">
+        <v>Work location</v>
+      </c>
+      <c r="L79" s="42" t="str">
+        <v>Tenure</v>
+      </c>
+      <c r="M79" s="42" t="str">
+        <v>Work Type</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13">
+      <c r="A80" t="str" cm="1">
+        <f t="array" ref="A80:F83">_xlfn._xlws.FILTER(staff[[Emp ID]:[Salary]],(staff[Salary]&gt;F67)*(staff[Gender]="Female"))</f>
+        <v>SQ02174</v>
+      </c>
+      <c r="B80" t="str">
+        <v>Sidoney</v>
+      </c>
+      <c r="C80" t="str">
+        <v>Yitzhok</v>
+      </c>
+      <c r="D80" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E80" t="str">
+        <v>Engineering</v>
+      </c>
+      <c r="F80">
+        <v>118442.54</v>
+      </c>
+      <c r="H80" s="36"/>
+    </row>
+    <row r="81" spans="1:15">
+      <c r="A81" t="str">
+        <v>SQ04612</v>
+      </c>
+      <c r="B81" t="str">
+        <v>Mick</v>
+      </c>
+      <c r="C81" t="str">
+        <v>Spraberry</v>
+      </c>
+      <c r="D81" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E81" t="str">
+        <v>Services</v>
+      </c>
+      <c r="F81">
+        <v>120000</v>
+      </c>
+      <c r="H81" s="36"/>
+    </row>
+    <row r="82" spans="1:15">
+      <c r="A82" t="str">
+        <v>VT04093</v>
+      </c>
+      <c r="B82" t="str">
+        <v>Prasanna</v>
+      </c>
+      <c r="C82" t="str">
+        <v>Lakshmi</v>
+      </c>
+      <c r="D82" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E82" t="str">
+        <v>Training</v>
+      </c>
+      <c r="F82">
+        <v>116767.63</v>
+      </c>
+      <c r="H82" s="36"/>
+    </row>
+    <row r="83" spans="1:15">
+      <c r="A83" t="str">
+        <v>VT04093</v>
+      </c>
+      <c r="B83" t="str">
+        <v>Baruna</v>
+      </c>
+      <c r="C83" t="str">
+        <v>Ogale</v>
+      </c>
+      <c r="D83" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E83" t="str">
+        <v>Training</v>
+      </c>
+      <c r="F83">
+        <v>116767.63</v>
+      </c>
+      <c r="H83" s="36"/>
+    </row>
+    <row r="84" spans="1:15">
+      <c r="H84" s="36"/>
+    </row>
+    <row r="85" spans="1:15" ht="21">
+      <c r="A85" s="30" t="s">
+        <v>779</v>
+      </c>
+      <c r="B85" s="30"/>
+      <c r="C85" s="30"/>
+      <c r="D85" s="30"/>
+      <c r="E85" s="30"/>
+      <c r="F85" s="30"/>
+      <c r="G85" s="30"/>
+      <c r="H85" s="30"/>
+      <c r="I85" s="30"/>
+      <c r="J85" s="30"/>
+      <c r="K85" s="30"/>
+      <c r="L85" s="30"/>
+      <c r="M85" s="30"/>
+      <c r="N85" s="30"/>
+      <c r="O85" s="30"/>
+    </row>
+    <row r="86" spans="1:15">
+      <c r="A86" s="42" t="str" cm="1">
+        <f t="array" ref="A86:M86">staff[#Headers]</f>
+        <v>Emp ID</v>
+      </c>
+      <c r="B86" s="42" t="str">
+        <v>First Name</v>
+      </c>
+      <c r="C86" s="42" t="str">
+        <v>Last Name</v>
+      </c>
+      <c r="D86" s="42" t="str">
+        <v>Gender</v>
+      </c>
+      <c r="E86" s="42" t="str">
+        <v>Department</v>
+      </c>
+      <c r="F86" s="42" t="str">
+        <v>Salary</v>
+      </c>
+      <c r="G86" s="42" t="str">
+        <v>Salary Bucket</v>
+      </c>
+      <c r="H86" s="43" t="str">
+        <v>Start Date</v>
+      </c>
+      <c r="I86" s="42" t="str">
+        <v>FTE</v>
+      </c>
+      <c r="J86" s="42" t="str">
+        <v>Employee type</v>
+      </c>
+      <c r="K86" s="42" t="str">
+        <v>Work location</v>
+      </c>
+      <c r="L86" s="42" t="str">
+        <v>Tenure</v>
+      </c>
+      <c r="M86" s="42" t="str">
+        <v>Work Type</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15">
+      <c r="A87" t="str" cm="1">
+        <f t="array" ref="A87:M90">_xlfn._xlws.FILTER(staff[],(staff[Salary]&gt;F67)*(staff[Gender]="Female")*(staff[Start Date] &gt; DATE(2019,12,31)))</f>
+        <v>SQ02174</v>
+      </c>
+      <c r="B87" t="str">
+        <v>Sidoney</v>
+      </c>
+      <c r="C87" t="str">
+        <v>Yitzhok</v>
+      </c>
+      <c r="D87" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E87" t="str">
+        <v>Engineering</v>
+      </c>
+      <c r="F87">
+        <v>118442.54</v>
+      </c>
+      <c r="G87" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H87" s="36">
+        <v>44193</v>
+      </c>
+      <c r="I87">
+        <v>1</v>
+      </c>
+      <c r="J87" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K87" t="str">
+        <v>Auckland, New Zealand</v>
+      </c>
+      <c r="L87">
+        <v>3.4821917808219176</v>
+      </c>
+      <c r="M87" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15">
+      <c r="A88" t="str">
+        <v>SQ04612</v>
+      </c>
+      <c r="B88" t="str">
+        <v>Mick</v>
+      </c>
+      <c r="C88" t="str">
+        <v>Spraberry</v>
+      </c>
+      <c r="D88" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E88" t="str">
+        <v>Services</v>
+      </c>
+      <c r="F88">
+        <v>120000</v>
+      </c>
+      <c r="G88" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H88" s="36">
+        <v>43902</v>
+      </c>
+      <c r="I88">
+        <v>0.9</v>
+      </c>
+      <c r="J88" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="K88" t="str">
+        <v>Remote</v>
+      </c>
+      <c r="L88">
+        <v>4.279452054794521</v>
+      </c>
+      <c r="M88" t="str">
+        <v>Part time</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15">
+      <c r="A89" t="str">
+        <v>VT04093</v>
+      </c>
+      <c r="B89" t="str">
+        <v>Prasanna</v>
+      </c>
+      <c r="C89" t="str">
+        <v>Lakshmi</v>
+      </c>
+      <c r="D89" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E89" t="str">
+        <v>Training</v>
+      </c>
+      <c r="F89">
+        <v>116767.63</v>
+      </c>
+      <c r="G89" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H89" s="36">
+        <v>43949</v>
+      </c>
+      <c r="I89">
+        <v>0.4</v>
+      </c>
+      <c r="J89" t="str">
+        <v>Temporary</v>
+      </c>
+      <c r="K89" t="str">
+        <v>Chennai, India</v>
+      </c>
+      <c r="L89">
+        <v>4.1506849315068495</v>
+      </c>
+      <c r="M89" t="str">
+        <v>Part time</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15">
+      <c r="A90" t="str">
+        <v>VT04093</v>
+      </c>
+      <c r="B90" t="str">
+        <v>Baruna</v>
+      </c>
+      <c r="C90" t="str">
+        <v>Ogale</v>
+      </c>
+      <c r="D90" t="str">
+        <v>Female</v>
+      </c>
+      <c r="E90" t="str">
+        <v>Training</v>
+      </c>
+      <c r="F90">
+        <v>116767.63</v>
+      </c>
+      <c r="G90" t="str">
+        <v>Above 100k</v>
+      </c>
+      <c r="H90" s="36">
+        <v>43949</v>
+      </c>
+      <c r="I90">
+        <v>0.4</v>
+      </c>
+      <c r="J90" t="str">
+        <v>Temporary</v>
+      </c>
+      <c r="K90" t="str">
+        <v>Chennai, India</v>
+      </c>
+      <c r="L90">
+        <v>4.1506849315068495</v>
+      </c>
+      <c r="M90" t="str">
+        <v>Part time</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15">
+      <c r="H91" s="36"/>
+    </row>
+    <row r="92" spans="1:15">
+      <c r="H92" s="36"/>
+    </row>
+    <row r="93" spans="1:15" ht="25.8">
+      <c r="A93" s="32" t="s">
+        <v>784</v>
+      </c>
+      <c r="B93" s="32"/>
+      <c r="C93" s="32"/>
+      <c r="D93" s="32"/>
+      <c r="E93" s="32"/>
+      <c r="F93" s="32"/>
+      <c r="G93" s="40"/>
+      <c r="H93" s="40"/>
+      <c r="I93" s="40"/>
+      <c r="J93" s="40"/>
+    </row>
+    <row r="94" spans="1:15">
+      <c r="H94" s="36"/>
+    </row>
+    <row r="95" spans="1:15">
+      <c r="B95" s="42" t="s">
+        <v>780</v>
+      </c>
+      <c r="C95" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D95" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="H95" s="36"/>
+    </row>
+    <row r="96" spans="1:15">
+      <c r="A96" s="7" t="s">
+        <v>781</v>
+      </c>
+      <c r="B96" s="46">
+        <f>MIN(staff[Salary])</f>
+        <v>28160.79</v>
+      </c>
+      <c r="C96" s="46">
+        <f>_xlfn.MINIFS(staff[Salary],staff[Gender],C95)</f>
+        <v>28160.79</v>
+      </c>
+      <c r="D96" s="46">
+        <f>_xlfn.MINIFS(staff[Salary],staff[Gender],D95)</f>
+        <v>28305.08</v>
+      </c>
+      <c r="H96" s="36"/>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="A97" s="7" t="s">
+        <v>782</v>
+      </c>
+      <c r="B97" s="46">
+        <f>MAX(staff[Salary])</f>
+        <v>120000</v>
+      </c>
+      <c r="C97" s="46">
+        <f>_xlfn.MAXIFS(staff[Salary],staff[Gender],C95)</f>
+        <v>120000</v>
+      </c>
+      <c r="D97" s="46">
+        <f>_xlfn.MAXIFS(staff[Salary],staff[Gender],D95)</f>
+        <v>120000</v>
+      </c>
+      <c r="H97" s="36"/>
+    </row>
+    <row r="98" spans="1:8">
+      <c r="A98" s="7" t="s">
+        <v>783</v>
+      </c>
+      <c r="B98" s="46">
+        <f>LARGE(staff[Salary],E98)</f>
+        <v>120000</v>
+      </c>
+      <c r="C98" s="46" cm="1">
+        <f t="array" ref="C98">LARGE(_xlfn._xlws.FILTER(staff[Salary],staff[Gender]="Male"),E98)</f>
+        <v>120000</v>
+      </c>
+      <c r="D98" s="46" cm="1">
+        <f t="array" ref="D98">LARGE(_xlfn._xlws.FILTER(staff[Salary],staff[Gender]=D95),E98)</f>
+        <v>120000</v>
+      </c>
+      <c r="E98">
+        <v>1</v>
+      </c>
+      <c r="H98" s="36"/>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="B99" s="46">
+        <f>LARGE(staff[Salary],E99)</f>
+        <v>120000</v>
+      </c>
+      <c r="C99" s="46" cm="1">
+        <f t="array" ref="C99">LARGE(_xlfn._xlws.FILTER(staff[Salary],staff[Gender]="Male"),E99)</f>
+        <v>119022.49</v>
+      </c>
+      <c r="D99" s="46" cm="1">
+        <f t="array" ref="D99">LARGE(_xlfn._xlws.FILTER(staff[Salary],staff[Gender]="Female"),E99)</f>
+        <v>118442.54</v>
+      </c>
+      <c r="E99">
+        <v>2</v>
+      </c>
+      <c r="H99" s="36"/>
+    </row>
+    <row r="100" spans="1:8">
+      <c r="B100" s="46">
+        <f>LARGE(staff[Salary],E100)</f>
+        <v>119022.49</v>
+      </c>
+      <c r="C100" s="46" cm="1">
+        <f t="array" ref="C100">LARGE(_xlfn._xlws.FILTER(staff[Salary],staff[Gender]="Male"),E100)</f>
+        <v>118976.16</v>
+      </c>
+      <c r="D100" s="46" cm="1">
+        <f t="array" ref="D100">LARGE(_xlfn._xlws.FILTER(staff[Salary],staff[Gender]="Female"),E100)</f>
+        <v>116767.63</v>
+      </c>
+      <c r="E100">
+        <v>3</v>
+      </c>
+      <c r="H100" s="36"/>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="B101" s="46">
+        <f>LARGE(staff[Salary],E101)</f>
+        <v>118976.16</v>
+      </c>
+      <c r="C101" s="46" cm="1">
+        <f t="array" ref="C101">LARGE(_xlfn._xlws.FILTER(staff[Salary],staff[Gender]="Male"),E101)</f>
+        <v>115191.38</v>
+      </c>
+      <c r="D101" s="46" cm="1">
+        <f t="array" ref="D101">LARGE(_xlfn._xlws.FILTER(staff[Salary],staff[Gender]="Female"),E101)</f>
+        <v>116767.63</v>
+      </c>
+      <c r="E101">
+        <v>4</v>
+      </c>
+      <c r="H101" s="36"/>
+    </row>
+    <row r="102" spans="1:8">
+      <c r="B102" s="46">
+        <f>LARGE(staff[Salary],E102)</f>
+        <v>118442.54</v>
+      </c>
+      <c r="C102" s="46" cm="1">
+        <f t="array" ref="C102">LARGE(_xlfn._xlws.FILTER(staff[Salary],staff[Gender]="Male"),E102)</f>
+        <v>114691.03</v>
+      </c>
+      <c r="D102" s="46" cm="1">
+        <f t="array" ref="D102">LARGE(_xlfn._xlws.FILTER(staff[Salary],staff[Gender]="Female"),E102)</f>
+        <v>114772.32</v>
+      </c>
+      <c r="E102">
+        <v>5</v>
+      </c>
+      <c r="H102" s="36"/>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="B103" s="47"/>
+      <c r="C103" s="47"/>
+      <c r="D103" s="47"/>
+      <c r="H103" s="36"/>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="A104" s="48" t="s">
+        <v>785</v>
+      </c>
+      <c r="B104" s="48"/>
+      <c r="C104" s="48"/>
+      <c r="D104" s="48"/>
+      <c r="H104" s="36"/>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="A105" t="s">
+        <v>789</v>
+      </c>
+      <c r="B105" s="46" t="e" cm="1">
+        <f t="array" aca="1" ref="B105" ca="1">TAKE(_xlfn._xlws.SORT(staff[Salary],,-1),5)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C105" s="46"/>
+      <c r="D105" s="46"/>
+      <c r="H105" s="36"/>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="B106" s="46"/>
+      <c r="C106" s="46"/>
+      <c r="D106" s="46"/>
+      <c r="H106" s="36"/>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="B107" s="46"/>
+      <c r="C107" s="46"/>
+      <c r="D107" s="46"/>
+      <c r="H107" s="36"/>
+    </row>
+    <row r="108" spans="1:8">
+      <c r="B108" s="46"/>
+      <c r="C108" s="46"/>
+      <c r="D108" s="46"/>
+      <c r="H108" s="36"/>
+    </row>
+    <row r="109" spans="1:8">
+      <c r="B109" s="46"/>
+      <c r="C109" s="46"/>
+      <c r="D109" s="46"/>
+      <c r="H109" s="36"/>
+    </row>
+    <row r="110" spans="1:8">
+      <c r="H110" s="36"/>
+    </row>
+    <row r="111" spans="1:8" ht="21">
+      <c r="A111" s="30" t="s">
+        <v>748</v>
+      </c>
+      <c r="B111" s="28"/>
+      <c r="C111" s="28"/>
+      <c r="D111" s="28"/>
+      <c r="H111" s="36"/>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="H112" s="36"/>
+    </row>
+    <row r="113" spans="1:8">
+      <c r="A113" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B113" t="s">
+        <v>786</v>
+      </c>
+      <c r="C113">
+        <f>COUNTA(_xlfn.ANCHORARRAY(A114))</f>
+        <v>12</v>
+      </c>
+      <c r="H113" s="36"/>
+    </row>
+    <row r="114" spans="1:8">
+      <c r="A114" t="str" cm="1">
+        <f t="array" ref="A114:A125">_xlfn.UNIQUE(staff[Department])</f>
+        <v>Training</v>
+      </c>
+      <c r="B114" t="str">
+        <f>_xlfn.TEXTJOIN(", ",TRUE,_xlfn.ANCHORARRAY(A114))</f>
+        <v>Training, Business Development, Engineering, Marketing, Legal, Accounting, Human Resources, Research and Development, Services, Product Management, Support, Sales</v>
+      </c>
+      <c r="H114" s="36"/>
+    </row>
+    <row r="115" spans="1:8">
+      <c r="A115" t="str">
+        <v>Business Development</v>
+      </c>
+      <c r="H115" s="36"/>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="A116" t="str">
+        <v>Engineering</v>
+      </c>
+      <c r="H116" s="36"/>
+    </row>
+    <row r="117" spans="1:8">
+      <c r="A117" t="str">
+        <v>Marketing</v>
+      </c>
+      <c r="H117" s="36"/>
+    </row>
+    <row r="118" spans="1:8">
+      <c r="A118" t="str">
+        <v>Legal</v>
+      </c>
+      <c r="H118" s="36"/>
+    </row>
+    <row r="119" spans="1:8">
+      <c r="A119" t="str">
+        <v>Accounting</v>
+      </c>
+      <c r="H119" s="36"/>
+    </row>
+    <row r="120" spans="1:8">
+      <c r="A120" t="str">
+        <v>Human Resources</v>
+      </c>
+      <c r="H120" s="36"/>
+    </row>
+    <row r="121" spans="1:8">
+      <c r="A121" t="str">
+        <v>Research and Development</v>
+      </c>
+      <c r="H121" s="36"/>
+    </row>
+    <row r="122" spans="1:8">
+      <c r="A122" t="str">
+        <v>Services</v>
+      </c>
+      <c r="H122" s="36"/>
+    </row>
+    <row r="123" spans="1:8">
+      <c r="A123" t="str">
+        <v>Product Management</v>
+      </c>
+      <c r="H123" s="36"/>
+    </row>
+    <row r="124" spans="1:8">
+      <c r="A124" t="str">
+        <v>Support</v>
+      </c>
+      <c r="H124" s="36"/>
+    </row>
+    <row r="125" spans="1:8">
+      <c r="A125" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="H125" s="36"/>
+    </row>
+    <row r="126" spans="1:8">
+      <c r="H126" s="36"/>
+    </row>
+    <row r="127" spans="1:8" ht="23.4">
+      <c r="A127" s="31" t="s">
+        <v>787</v>
+      </c>
+      <c r="B127" s="31"/>
+      <c r="C127" s="31"/>
+      <c r="D127" s="31"/>
+      <c r="E127" s="31"/>
+      <c r="F127" s="31"/>
+      <c r="H127" s="36"/>
+    </row>
+    <row r="128" spans="1:8">
+      <c r="A128" t="s">
+        <v>788</v>
+      </c>
+      <c r="B128" s="41" t="s">
+        <v>501</v>
+      </c>
+      <c r="H128" s="36"/>
+    </row>
+    <row r="129" spans="1:19">
+      <c r="H129" s="36"/>
+    </row>
+    <row r="130" spans="1:19" ht="15" thickBot="1">
+      <c r="A130" t="s">
+        <v>1</v>
+      </c>
+      <c r="B130" s="49" t="str">
+        <f>IFERROR(VLOOKUP($B$128,staff[],C130,FALSE),"Not Found")</f>
+        <v>Edd</v>
+      </c>
+      <c r="C130" s="51">
+        <v>2</v>
+      </c>
+      <c r="D130" t="str">
+        <f>_xlfn.XLOOKUP(B128,staff[Emp ID],staff[First Name],"Not Found",0,1)</f>
+        <v>Edd</v>
+      </c>
+      <c r="H130" s="36"/>
+    </row>
+    <row r="131" spans="1:19" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A131" t="s">
+        <v>2</v>
+      </c>
+      <c r="B131" s="49" t="str">
+        <f>IFERROR(VLOOKUP($B$128,staff[],C131,FALSE),"Not Found")</f>
+        <v>MacKnockiter</v>
+      </c>
+      <c r="C131" s="51">
+        <v>3</v>
+      </c>
+      <c r="H131" s="36"/>
+    </row>
+    <row r="132" spans="1:19" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A132" t="s">
+        <v>4</v>
+      </c>
+      <c r="B132" s="49" t="str">
+        <f>IFERROR(VLOOKUP($B$128,staff[],C132,FALSE),"Not Found")</f>
+        <v>Accounting</v>
+      </c>
+      <c r="C132" s="51">
+        <v>5</v>
+      </c>
+      <c r="H132" s="36"/>
+    </row>
+    <row r="133" spans="1:19" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A133" t="s">
+        <v>5</v>
+      </c>
+      <c r="B133" s="49">
+        <f>IFERROR(VLOOKUP($B$128,staff[],C133,FALSE),"Not Found")</f>
+        <v>119022.49</v>
+      </c>
+      <c r="C133" s="51">
+        <v>6</v>
+      </c>
+      <c r="H133" s="36"/>
+    </row>
+    <row r="134" spans="1:19" ht="15" thickTop="1">
+      <c r="H134" s="36"/>
+    </row>
+    <row r="135" spans="1:19" ht="23.4">
+      <c r="A135" s="31" t="s">
+        <v>790</v>
+      </c>
+      <c r="B135" s="31"/>
+      <c r="C135" s="31"/>
+      <c r="D135" s="31"/>
+      <c r="E135" s="31"/>
+      <c r="F135" s="31"/>
+      <c r="H135" s="36"/>
+    </row>
+    <row r="136" spans="1:19">
+      <c r="H136" s="36"/>
+    </row>
+    <row r="137" spans="1:19">
+      <c r="A137" t="s">
+        <v>791</v>
+      </c>
+      <c r="B137" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="D137" s="50"/>
+      <c r="E137" s="41" t="s">
+        <v>792</v>
+      </c>
+      <c r="G137" s="41" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="138" spans="1:19">
+      <c r="B138">
+        <f>MATCH(B137,staff[Last Name],0)</f>
+        <v>43</v>
+      </c>
+      <c r="G138" t="str" cm="1">
+        <f t="array" ref="G138:S138">_xlfn.XLOOKUP(B137,staff[Last Name],staff[])</f>
+        <v>PR03532</v>
+      </c>
+      <c r="H138" t="str">
+        <v>Crawford</v>
+      </c>
+      <c r="I138" t="str">
+        <v>Scad</v>
+      </c>
+      <c r="J138" t="str">
+        <v>Male</v>
+      </c>
+      <c r="K138" t="str">
+        <v>Human Resources</v>
+      </c>
+      <c r="L138">
+        <v>72876.91</v>
+      </c>
+      <c r="M138" t="str">
+        <v>50k to 100k</v>
+      </c>
+      <c r="N138">
+        <v>43837</v>
+      </c>
+      <c r="O138">
+        <v>1</v>
+      </c>
+      <c r="P138" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="Q138" t="str">
+        <v>Remote</v>
+      </c>
+      <c r="R138">
+        <v>4.4575342465753423</v>
+      </c>
+      <c r="S138" t="str">
+        <v>Full time</v>
+      </c>
+    </row>
+    <row r="139" spans="1:19" ht="15" thickBot="1">
+      <c r="A139" t="s">
+        <v>788</v>
+      </c>
+      <c r="B139" s="49" t="str" cm="1">
+        <f t="array" ref="B139">INDEX(staff[Emp ID],B138)</f>
+        <v>PR03532</v>
+      </c>
+      <c r="D139" t="s">
+        <v>1</v>
+      </c>
+      <c r="E139" t="str">
+        <f>_xlfn.XLOOKUP(B128,staff[Emp ID],staff[First Name],"Not Found")</f>
+        <v>Edd</v>
+      </c>
+      <c r="G139" t="str" cm="1">
+        <f t="array" ref="G139:G151">TRANSPOSE(_xlfn.XLOOKUP(B137,staff[Last Name],staff[]))</f>
+        <v>PR03532</v>
+      </c>
+    </row>
+    <row r="140" spans="1:19" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A140" t="s">
+        <v>4</v>
+      </c>
+      <c r="B140" s="49" t="str" cm="1">
+        <f t="array" ref="B140">INDEX(staff[Department],B138)</f>
+        <v>Human Resources</v>
+      </c>
+      <c r="D140" t="s">
+        <v>2</v>
+      </c>
+      <c r="E140" t="str">
+        <f>_xlfn.XLOOKUP(B128,staff[Emp ID],staff[Last Name],"Not Found")</f>
+        <v>MacKnockiter</v>
+      </c>
+      <c r="G140" t="str">
+        <v>Crawford</v>
+      </c>
+    </row>
+    <row r="141" spans="1:19" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A141" t="s">
+        <v>5</v>
+      </c>
+      <c r="B141" s="49" cm="1">
+        <f t="array" ref="B141">INDEX(staff[Salary],B138)</f>
+        <v>72876.91</v>
+      </c>
+      <c r="D141" t="s">
+        <v>4</v>
+      </c>
+      <c r="E141" t="str">
+        <f>_xlfn.XLOOKUP(B128,staff[Emp ID],staff[Department],"Not Found")</f>
+        <v>Accounting</v>
+      </c>
+      <c r="G141" t="str">
+        <v>Scad</v>
+      </c>
+    </row>
+    <row r="142" spans="1:19" ht="15" thickTop="1">
+      <c r="D142" t="s">
+        <v>5</v>
+      </c>
+      <c r="E142">
+        <f>_xlfn.XLOOKUP(B128,staff[Emp ID],staff[Salary],"Not Found",0,1)</f>
+        <v>119022.49</v>
+      </c>
+      <c r="G142" t="str">
+        <v>Male</v>
+      </c>
+    </row>
+    <row r="143" spans="1:19">
+      <c r="G143" t="str">
+        <v>Human Resources</v>
+      </c>
+      <c r="H143" s="36"/>
+    </row>
+    <row r="144" spans="1:19">
+      <c r="G144">
+        <v>72876.91</v>
+      </c>
+      <c r="H144" s="36"/>
+    </row>
+    <row r="145" spans="1:8">
+      <c r="G145" t="str">
+        <v>50k to 100k</v>
+      </c>
+      <c r="H145" s="36"/>
+    </row>
+    <row r="146" spans="1:8">
+      <c r="G146">
+        <v>43837</v>
+      </c>
+      <c r="H146" s="36"/>
+    </row>
+    <row r="147" spans="1:8">
+      <c r="G147">
+        <v>1</v>
+      </c>
+      <c r="H147" s="36"/>
+    </row>
+    <row r="148" spans="1:8">
+      <c r="G148" t="str">
+        <v>Permanent</v>
+      </c>
+      <c r="H148" s="36"/>
+    </row>
+    <row r="149" spans="1:8">
+      <c r="G149" t="str">
+        <v>Remote</v>
+      </c>
+      <c r="H149" s="36"/>
+    </row>
+    <row r="150" spans="1:8">
+      <c r="G150">
+        <v>4.4575342465753423</v>
+      </c>
+      <c r="H150" s="36"/>
+    </row>
+    <row r="151" spans="1:8">
+      <c r="A151" s="39" t="s">
+        <v>765</v>
+      </c>
+      <c r="G151" t="str">
+        <v>Full time</v>
+      </c>
+      <c r="H151" s="36"/>
+    </row>
+    <row r="152" spans="1:8">
+      <c r="A152" t="e" cm="1" vm="1">
+        <f t="array" ref="A152">_xlfn._xlws.FILTER(staff[],staff[Salary]&gt;120000)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B152" t="s">
+        <v>793</v>
+      </c>
+      <c r="H152" s="36"/>
+    </row>
+    <row r="153" spans="1:8">
+      <c r="H153" s="36"/>
+    </row>
+    <row r="154" spans="1:8">
+      <c r="H154" s="36"/>
+    </row>
+    <row r="155" spans="1:8">
+      <c r="H155" s="36"/>
+    </row>
+    <row r="156" spans="1:8">
+      <c r="H156" s="36"/>
+    </row>
+    <row r="157" spans="1:8">
+      <c r="H157" s="36"/>
+    </row>
+    <row r="158" spans="1:8">
+      <c r="H158" s="36"/>
+    </row>
+    <row r="159" spans="1:8">
+      <c r="H159" s="36"/>
+    </row>
+    <row r="160" spans="1:8">
+      <c r="H160" s="36"/>
+    </row>
+    <row r="161" spans="8:8">
+      <c r="H161" s="36"/>
+    </row>
+    <row r="162" spans="8:8">
+      <c r="H162" s="36"/>
+    </row>
+    <row r="163" spans="8:8">
+      <c r="H163" s="36"/>
+    </row>
+    <row r="164" spans="8:8">
+      <c r="H164" s="36"/>
+    </row>
+    <row r="165" spans="8:8">
+      <c r="H165" s="36"/>
+    </row>
+    <row r="166" spans="8:8">
+      <c r="H166" s="36"/>
+    </row>
+    <row r="167" spans="8:8">
+      <c r="H167" s="36"/>
+    </row>
+    <row r="168" spans="8:8">
+      <c r="H168" s="36"/>
+    </row>
+    <row r="169" spans="8:8">
+      <c r="H169" s="36"/>
+    </row>
+    <row r="170" spans="8:8">
+      <c r="H170" s="36"/>
+    </row>
+    <row r="171" spans="8:8">
+      <c r="H171" s="36"/>
+    </row>
+    <row r="172" spans="8:8">
+      <c r="H172" s="36"/>
+    </row>
+    <row r="173" spans="8:8">
+      <c r="H173" s="36"/>
+    </row>
+    <row r="174" spans="8:8">
+      <c r="H174" s="36"/>
+    </row>
+    <row r="175" spans="8:8">
+      <c r="H175" s="36"/>
+    </row>
+    <row r="176" spans="8:8">
+      <c r="H176" s="36"/>
+    </row>
+    <row r="177" spans="8:8">
+      <c r="H177" s="36"/>
+    </row>
+    <row r="178" spans="8:8">
+      <c r="H178" s="36"/>
+    </row>
+    <row r="179" spans="8:8">
+      <c r="H179" s="36"/>
+    </row>
+    <row r="180" spans="8:8">
+      <c r="H180" s="36"/>
+    </row>
+    <row r="181" spans="8:8">
+      <c r="H181" s="36"/>
+    </row>
+    <row r="182" spans="8:8">
+      <c r="H182" s="36"/>
+    </row>
+    <row r="183" spans="8:8">
+      <c r="H183" s="36"/>
+    </row>
+    <row r="184" spans="8:8">
+      <c r="H184" s="36"/>
+    </row>
+    <row r="185" spans="8:8">
+      <c r="H185" s="36"/>
+    </row>
+    <row r="186" spans="8:8">
+      <c r="H186" s="36"/>
+    </row>
+    <row r="187" spans="8:8">
+      <c r="H187" s="36"/>
+    </row>
+    <row r="188" spans="8:8">
+      <c r="H188" s="36"/>
+    </row>
+    <row r="189" spans="8:8">
+      <c r="H189" s="36"/>
+    </row>
+    <row r="190" spans="8:8">
+      <c r="H190" s="36"/>
+    </row>
+    <row r="191" spans="8:8">
+      <c r="H191" s="36"/>
+    </row>
+    <row r="192" spans="8:8">
+      <c r="H192" s="36"/>
+    </row>
+    <row r="193" spans="8:8">
+      <c r="H193" s="36"/>
+    </row>
+    <row r="194" spans="8:8">
+      <c r="H194" s="36"/>
+    </row>
+    <row r="195" spans="8:8">
+      <c r="H195" s="36"/>
+    </row>
+    <row r="196" spans="8:8">
+      <c r="H196" s="36"/>
+    </row>
+    <row r="197" spans="8:8">
+      <c r="H197" s="36"/>
+    </row>
+    <row r="198" spans="8:8">
+      <c r="H198" s="36"/>
+    </row>
+    <row r="199" spans="8:8">
+      <c r="H199" s="36"/>
+    </row>
+    <row r="200" spans="8:8">
+      <c r="H200" s="36"/>
+    </row>
+    <row r="201" spans="8:8">
+      <c r="H201" s="36"/>
+    </row>
+    <row r="202" spans="8:8">
+      <c r="H202" s="36"/>
+    </row>
+    <row r="203" spans="8:8">
+      <c r="H203" s="36"/>
+    </row>
+    <row r="204" spans="8:8">
+      <c r="H204" s="36"/>
+    </row>
+    <row r="205" spans="8:8">
+      <c r="H205" s="36"/>
+    </row>
+    <row r="206" spans="8:8">
+      <c r="H206" s="36"/>
+    </row>
+    <row r="207" spans="8:8">
+      <c r="H207" s="36"/>
+    </row>
+    <row r="208" spans="8:8">
+      <c r="H208" s="36"/>
+    </row>
+    <row r="209" spans="8:8">
+      <c r="H209" s="36"/>
+    </row>
+    <row r="210" spans="8:8">
+      <c r="H210" s="36"/>
+    </row>
+    <row r="211" spans="8:8">
+      <c r="H211" s="36"/>
+    </row>
+    <row r="212" spans="8:8">
+      <c r="H212" s="36"/>
+    </row>
+    <row r="213" spans="8:8">
+      <c r="H213" s="36"/>
+    </row>
+    <row r="214" spans="8:8">
+      <c r="H214" s="36"/>
+    </row>
+    <row r="215" spans="8:8">
+      <c r="H215" s="36"/>
+    </row>
+    <row r="216" spans="8:8">
+      <c r="H216" s="36"/>
+    </row>
+    <row r="217" spans="8:8">
+      <c r="H217" s="36"/>
+    </row>
+    <row r="218" spans="8:8">
+      <c r="H218" s="36"/>
+    </row>
+    <row r="219" spans="8:8">
+      <c r="H219" s="36"/>
+    </row>
+    <row r="220" spans="8:8">
+      <c r="H220" s="36"/>
+    </row>
+    <row r="221" spans="8:8">
+      <c r="H221" s="36"/>
+    </row>
+    <row r="222" spans="8:8">
+      <c r="H222" s="36"/>
+    </row>
+    <row r="223" spans="8:8">
+      <c r="H223" s="36"/>
+    </row>
+    <row r="224" spans="8:8">
+      <c r="H224" s="36"/>
+    </row>
+    <row r="225" spans="8:8">
+      <c r="H225" s="36"/>
+    </row>
+    <row r="226" spans="8:8">
+      <c r="H226" s="36"/>
+    </row>
+    <row r="227" spans="8:8">
+      <c r="H227" s="36"/>
+    </row>
+    <row r="228" spans="8:8">
+      <c r="H228" s="36"/>
+    </row>
+    <row r="229" spans="8:8">
+      <c r="H229" s="36"/>
+    </row>
+    <row r="230" spans="8:8">
+      <c r="H230" s="36"/>
+    </row>
+    <row r="231" spans="8:8">
+      <c r="H231" s="36"/>
+    </row>
+    <row r="232" spans="8:8">
+      <c r="H232" s="36"/>
+    </row>
+    <row r="233" spans="8:8">
+      <c r="H233" s="36"/>
+    </row>
+    <row r="234" spans="8:8">
+      <c r="H234" s="36"/>
+    </row>
+    <row r="235" spans="8:8">
+      <c r="H235" s="36"/>
+    </row>
+    <row r="236" spans="8:8">
+      <c r="H236" s="36"/>
+    </row>
+    <row r="237" spans="8:8">
+      <c r="H237" s="36"/>
+    </row>
+    <row r="238" spans="8:8">
+      <c r="H238" s="36"/>
+    </row>
+    <row r="239" spans="8:8">
+      <c r="H239" s="36"/>
+    </row>
+    <row r="240" spans="8:8">
+      <c r="H240" s="36"/>
+    </row>
+    <row r="241" spans="8:8">
+      <c r="H241" s="36"/>
+    </row>
+    <row r="242" spans="8:8">
+      <c r="H242" s="36"/>
+    </row>
+    <row r="243" spans="8:8">
+      <c r="H243" s="36"/>
+    </row>
+    <row r="244" spans="8:8">
+      <c r="H244" s="36"/>
+    </row>
+    <row r="245" spans="8:8">
+      <c r="H245" s="36"/>
+    </row>
+    <row r="246" spans="8:8">
+      <c r="H246" s="36"/>
+    </row>
+    <row r="247" spans="8:8">
+      <c r="H247" s="36"/>
+    </row>
+    <row r="248" spans="8:8">
+      <c r="H248" s="36"/>
+    </row>
+    <row r="249" spans="8:8">
+      <c r="H249" s="36"/>
+    </row>
+    <row r="250" spans="8:8">
+      <c r="H250" s="36"/>
+    </row>
+    <row r="251" spans="8:8">
+      <c r="H251" s="36"/>
+    </row>
+    <row r="252" spans="8:8">
+      <c r="H252" s="36"/>
+    </row>
+    <row r="253" spans="8:8">
+      <c r="H253" s="36"/>
+    </row>
+    <row r="254" spans="8:8">
+      <c r="H254" s="36"/>
+    </row>
+    <row r="255" spans="8:8">
+      <c r="H255" s="36"/>
+    </row>
+    <row r="256" spans="8:8">
+      <c r="H256" s="36"/>
+    </row>
+    <row r="257" spans="8:8">
+      <c r="H257" s="36"/>
+    </row>
+    <row r="258" spans="8:8">
+      <c r="H258" s="36"/>
+    </row>
+    <row r="259" spans="8:8">
+      <c r="H259" s="36"/>
+    </row>
+    <row r="260" spans="8:8">
+      <c r="H260" s="36"/>
+    </row>
+    <row r="261" spans="8:8">
+      <c r="H261" s="36"/>
+    </row>
+    <row r="262" spans="8:8">
+      <c r="H262" s="36"/>
+    </row>
+    <row r="263" spans="8:8">
+      <c r="H263" s="36"/>
+    </row>
+    <row r="264" spans="8:8">
+      <c r="H264" s="36"/>
+    </row>
+    <row r="265" spans="8:8">
+      <c r="H265" s="36"/>
+    </row>
+    <row r="266" spans="8:8">
+      <c r="H266" s="36"/>
+    </row>
+    <row r="267" spans="8:8">
+      <c r="H267" s="36"/>
+    </row>
+    <row r="268" spans="8:8">
+      <c r="H268" s="36"/>
+    </row>
+    <row r="269" spans="8:8">
+      <c r="H269" s="36"/>
+    </row>
+    <row r="270" spans="8:8">
+      <c r="H270" s="36"/>
+    </row>
+    <row r="271" spans="8:8">
+      <c r="H271" s="36"/>
+    </row>
+    <row r="272" spans="8:8">
+      <c r="H272" s="36"/>
+    </row>
+    <row r="273" spans="8:8">
+      <c r="H273" s="36"/>
+    </row>
+    <row r="274" spans="8:8">
+      <c r="H274" s="36"/>
+    </row>
+    <row r="275" spans="8:8">
+      <c r="H275" s="36"/>
+    </row>
+    <row r="276" spans="8:8">
+      <c r="H276" s="36"/>
+    </row>
+    <row r="277" spans="8:8">
+      <c r="H277" s="36"/>
+    </row>
+    <row r="278" spans="8:8">
+      <c r="H278" s="36"/>
+    </row>
   </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A127:F127"/>
+    <mergeCell ref="A135:F135"/>
+    <mergeCell ref="A85:O85"/>
+    <mergeCell ref="A104:D104"/>
+    <mergeCell ref="A93:F93"/>
+    <mergeCell ref="A111:D111"/>
+    <mergeCell ref="A66:G66"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="A78:L78"/>
+    <mergeCell ref="A16:M16"/>
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>